<commit_message>
less variations for root inputs
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_05.xlsx
+++ b/simulations/inputs/Scenarios_24_05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sshfs\torisuten@192.168.12.9\pp\Wheat-BRIDGES\Root_BRIDGES\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792C4C1F-5489-4F2C-9615-C7C2EC5AED64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612D69FA-8E65-410D-A9DE-1B6925AE7B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2302,7 +2302,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2500,7 +2500,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2510,7 +2510,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2835,8 +2834,8 @@
   <dimension ref="A1:K218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B223" sqref="B223"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5987,7 +5986,7 @@
         <v>0.05</v>
       </c>
       <c r="H90" s="77">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="I90" s="77">
         <v>0.05</v>
@@ -10392,10 +10391,10 @@
       <c r="D215" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="E215" s="101" t="s">
+      <c r="E215" s="96" t="s">
         <v>527</v>
       </c>
-      <c r="F215" s="101" t="s">
+      <c r="F215" s="96" t="s">
         <v>511</v>
       </c>
       <c r="G215" s="100">
@@ -10427,10 +10426,10 @@
       <c r="D216" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="E216" s="101" t="s">
+      <c r="E216" s="96" t="s">
         <v>529</v>
       </c>
-      <c r="F216" s="101" t="s">
+      <c r="F216" s="96" t="s">
         <v>530</v>
       </c>
       <c r="G216" s="99">
@@ -10467,10 +10466,10 @@
       <c r="D217" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="E217" s="101" t="s">
+      <c r="E217" s="96" t="s">
         <v>532</v>
       </c>
-      <c r="F217" s="101" t="s">
+      <c r="F217" s="96" t="s">
         <v>533</v>
       </c>
       <c r="G217" s="100">
@@ -10502,10 +10501,10 @@
       <c r="D218" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="E218" s="101" t="s">
+      <c r="E218" s="96" t="s">
         <v>535</v>
       </c>
-      <c r="F218" s="101" t="s">
+      <c r="F218" s="96" t="s">
         <v>536</v>
       </c>
       <c r="G218" s="99">

</xml_diff>

<commit_message>
mistake in root hairs growth
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_05.xlsx
+++ b/simulations/inputs/Scenarios_24_05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB77C309-12FE-4173-85DA-EE6D7DCA1910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB7425D-4008-4C6C-BBBF-FC6EF7476DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="540">
   <si>
     <t>input_file</t>
   </si>
@@ -1648,6 +1648,12 @@
   </si>
   <si>
     <t>Drew_temperature_si.csv</t>
+  </si>
+  <si>
+    <t>no_root_hairs_patch</t>
+  </si>
+  <si>
+    <t>no_root_hairs</t>
   </si>
 </sst>
 </file>
@@ -2834,11 +2840,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K218"/>
+  <dimension ref="A1:M218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K78" sqref="K78"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2848,10 +2854,10 @@
     <col min="5" max="5" width="58.109375" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" style="37" customWidth="1"/>
-    <col min="8" max="11" width="39.88671875" style="1" customWidth="1"/>
+    <col min="8" max="13" width="39.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>469</v>
       </c>
@@ -2885,8 +2891,14 @@
       <c r="K1" s="97" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="97" t="s">
+        <v>538</v>
+      </c>
+      <c r="M1" s="97" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>472</v>
       </c>
@@ -2920,8 +2932,14 @@
       <c r="K2" s="36" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="36" t="s">
+        <v>489</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>484</v>
       </c>
@@ -2955,8 +2973,14 @@
       <c r="K3" s="36" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="36" t="s">
+        <v>482</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>483</v>
       </c>
@@ -2990,8 +3014,14 @@
       <c r="K4" s="36" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="36" t="s">
+        <v>494</v>
+      </c>
+      <c r="M4" s="36" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>490</v>
       </c>
@@ -3025,8 +3055,14 @@
       <c r="K5" s="36" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="36" t="s">
+        <v>537</v>
+      </c>
+      <c r="M5" s="36" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>485</v>
       </c>
@@ -3060,8 +3096,14 @@
       <c r="K6" s="36" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="36" t="s">
+        <v>494</v>
+      </c>
+      <c r="M6" s="36" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -3095,8 +3137,14 @@
       <c r="K7" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -3130,8 +3178,14 @@
       <c r="K8" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="77">
+        <v>1</v>
+      </c>
+      <c r="M8" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="74" t="s">
         <v>444</v>
       </c>
@@ -3165,8 +3219,14 @@
       <c r="K9" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -3200,8 +3260,14 @@
       <c r="K10" s="85">
         <v>180</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="85">
+        <v>180</v>
+      </c>
+      <c r="M10" s="85">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -3235,8 +3301,14 @@
       <c r="K11" s="78">
         <v>4.1666666999999998E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11" s="78">
+        <v>4.1666666999999998E-2</v>
+      </c>
+      <c r="M11" s="78">
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
@@ -3270,8 +3342,14 @@
       <c r="K12" s="79">
         <v>4.1666666999999998E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12" s="79">
+        <v>4.1666666999999998E-2</v>
+      </c>
+      <c r="M12" s="79">
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>1</v>
       </c>
@@ -3305,8 +3383,14 @@
       <c r="K13" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13" s="77">
+        <v>1</v>
+      </c>
+      <c r="M13" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>448</v>
       </c>
@@ -3340,8 +3424,14 @@
       <c r="K14" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14" s="77">
+        <v>0</v>
+      </c>
+      <c r="M14" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>6</v>
       </c>
@@ -3375,8 +3465,14 @@
       <c r="K15" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>7</v>
       </c>
@@ -3410,8 +3506,14 @@
       <c r="K16" s="80">
         <v>5.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="80">
+        <v>5.0000000000000001E-9</v>
+      </c>
+      <c r="M16" s="80">
+        <v>5.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
@@ -3445,8 +3547,14 @@
       <c r="K17" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="77">
+        <v>10</v>
+      </c>
+      <c r="M17" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>461</v>
       </c>
@@ -3480,8 +3588,14 @@
       <c r="K18" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M18" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>462</v>
       </c>
@@ -3515,8 +3629,14 @@
       <c r="K19" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M19" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>465</v>
       </c>
@@ -3550,8 +3670,14 @@
       <c r="K20" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M20" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>467</v>
       </c>
@@ -3585,8 +3711,14 @@
       <c r="K21" s="77">
         <v>86400</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" s="77">
+        <v>86400</v>
+      </c>
+      <c r="M21" s="77">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>10</v>
       </c>
@@ -3620,8 +3752,14 @@
       <c r="K22" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="M22" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>11</v>
       </c>
@@ -3655,8 +3793,14 @@
       <c r="K23" s="77">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23" s="77">
+        <v>3</v>
+      </c>
+      <c r="M23" s="77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>363</v>
       </c>
@@ -3690,8 +3834,14 @@
       <c r="K24" s="81" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="M24" s="81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>365</v>
       </c>
@@ -3725,8 +3875,14 @@
       <c r="K25" s="81" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="M25" s="81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>377</v>
       </c>
@@ -3760,8 +3916,14 @@
       <c r="K26" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M26" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>376</v>
       </c>
@@ -3795,8 +3957,14 @@
       <c r="K27" s="81" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="M27" s="81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>375</v>
       </c>
@@ -3830,8 +3998,14 @@
       <c r="K28" s="81" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="M28" s="81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>12</v>
       </c>
@@ -3865,8 +4039,14 @@
       <c r="K29" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M29" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>13</v>
       </c>
@@ -3900,8 +4080,14 @@
       <c r="K30" s="77">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30" s="77">
+        <v>0.33</v>
+      </c>
+      <c r="M30" s="77">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>14</v>
       </c>
@@ -3935,8 +4121,14 @@
       <c r="K31" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M31" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>9</v>
       </c>
@@ -3970,8 +4162,14 @@
       <c r="K32" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M32" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>454</v>
       </c>
@@ -4005,8 +4203,14 @@
       <c r="K33" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M33" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>21</v>
       </c>
@@ -4040,8 +4244,14 @@
       <c r="K34" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="M34" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>22</v>
       </c>
@@ -4075,8 +4285,14 @@
       <c r="K35" s="85" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35" s="85" t="s">
+        <v>433</v>
+      </c>
+      <c r="M35" s="85" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>23</v>
       </c>
@@ -4110,8 +4326,14 @@
       <c r="K36" s="80">
         <v>9.9999999999999995E-7</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36" s="80">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M36" s="80">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>24</v>
       </c>
@@ -4145,8 +4367,14 @@
       <c r="K37" s="86">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37" s="86">
+        <v>1E-3</v>
+      </c>
+      <c r="M37" s="86">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>25</v>
       </c>
@@ -4180,8 +4408,14 @@
       <c r="K38" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="M38" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>26</v>
       </c>
@@ -4215,8 +4449,14 @@
       <c r="K39" s="77" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="M39" s="77" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>27</v>
       </c>
@@ -4250,8 +4490,14 @@
       <c r="K40" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="M40" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>28</v>
       </c>
@@ -4285,8 +4531,14 @@
       <c r="K41" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M41" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>29</v>
       </c>
@@ -4320,8 +4572,14 @@
       <c r="K42" s="77">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42" s="77">
+        <v>120</v>
+      </c>
+      <c r="M42" s="77">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>30</v>
       </c>
@@ -4355,8 +4613,14 @@
       <c r="K43" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43" s="77">
+        <v>0</v>
+      </c>
+      <c r="M43" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>31</v>
       </c>
@@ -4390,8 +4654,14 @@
       <c r="K44" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L44" s="77">
+        <v>0</v>
+      </c>
+      <c r="M44" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>32</v>
       </c>
@@ -4425,8 +4695,14 @@
       <c r="K45" s="77">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L45" s="77">
+        <v>-0.1</v>
+      </c>
+      <c r="M45" s="77">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>33</v>
       </c>
@@ -4460,8 +4736,14 @@
       <c r="K46" s="77">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L46" s="77">
+        <v>-0.2</v>
+      </c>
+      <c r="M46" s="77">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>34</v>
       </c>
@@ -4495,8 +4777,14 @@
       <c r="K47" s="77">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L47" s="77">
+        <v>0.4</v>
+      </c>
+      <c r="M47" s="77">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>35</v>
       </c>
@@ -4530,8 +4818,14 @@
       <c r="K48" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L48" s="77">
+        <v>0</v>
+      </c>
+      <c r="M48" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>434</v>
       </c>
@@ -4565,8 +4859,14 @@
       <c r="K49" s="77">
         <v>1200</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L49" s="77">
+        <v>1200</v>
+      </c>
+      <c r="M49" s="77">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>435</v>
       </c>
@@ -4600,8 +4900,14 @@
       <c r="K50" s="77">
         <v>1200</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L50" s="77">
+        <v>1200</v>
+      </c>
+      <c r="M50" s="77">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>457</v>
       </c>
@@ -4635,8 +4941,14 @@
       <c r="K51" s="35" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L51" s="35" t="s">
+        <v>460</v>
+      </c>
+      <c r="M51" s="35" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>15</v>
       </c>
@@ -4670,8 +4982,14 @@
       <c r="K52" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="M52" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>16</v>
       </c>
@@ -4705,8 +5023,14 @@
       <c r="K53" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L53" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="M53" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>17</v>
       </c>
@@ -4740,8 +5064,14 @@
       <c r="K54" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54" s="77">
+        <v>0</v>
+      </c>
+      <c r="M54" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>18</v>
       </c>
@@ -4775,8 +5105,14 @@
       <c r="K55" s="77">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L55" s="77">
+        <v>0.5</v>
+      </c>
+      <c r="M55" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>19</v>
       </c>
@@ -4810,8 +5146,14 @@
       <c r="K56" s="77">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56" s="77">
+        <v>0.05</v>
+      </c>
+      <c r="M56" s="77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
         <v>36</v>
       </c>
@@ -4845,8 +5187,14 @@
       <c r="K57" s="80">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57" s="80">
+        <v>1E-3</v>
+      </c>
+      <c r="M57" s="80">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
         <v>380</v>
       </c>
@@ -4880,8 +5228,14 @@
       <c r="K58" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58" s="77">
+        <v>0</v>
+      </c>
+      <c r="M58" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
         <v>37</v>
       </c>
@@ -4915,8 +5269,14 @@
       <c r="K59" s="77">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59" s="77">
+        <v>1E-4</v>
+      </c>
+      <c r="M59" s="77">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
         <v>38</v>
       </c>
@@ -4950,8 +5310,14 @@
       <c r="K60" s="77">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L60" s="77">
+        <v>1E-4</v>
+      </c>
+      <c r="M60" s="77">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="17" t="s">
         <v>39</v>
       </c>
@@ -4985,8 +5351,14 @@
       <c r="K61" s="77">
         <v>6.9999999999999999E-4</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L61" s="77">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="M61" s="77">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
         <v>40</v>
       </c>
@@ -5020,8 +5392,14 @@
       <c r="K62" s="77">
         <v>1.22E-4</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L62" s="77">
+        <v>1.22E-4</v>
+      </c>
+      <c r="M62" s="77">
+        <v>1.22E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
         <v>207</v>
       </c>
@@ -5055,8 +5433,14 @@
       <c r="K63" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L63" s="77">
+        <v>1</v>
+      </c>
+      <c r="M63" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>41</v>
       </c>
@@ -5090,8 +5474,14 @@
       <c r="K64" s="77">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L64" s="77">
+        <v>0.95</v>
+      </c>
+      <c r="M64" s="77">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
         <v>406</v>
       </c>
@@ -5125,8 +5515,14 @@
       <c r="K65" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L65" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M65" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>91</v>
       </c>
@@ -5160,8 +5556,14 @@
       <c r="K66" s="77">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L66" s="77">
+        <v>5</v>
+      </c>
+      <c r="M66" s="77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
         <v>408</v>
       </c>
@@ -5195,8 +5597,14 @@
       <c r="K67" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L67" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M67" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
         <v>42</v>
       </c>
@@ -5230,8 +5638,14 @@
       <c r="K68" s="77">
         <v>50</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L68" s="77">
+        <v>50</v>
+      </c>
+      <c r="M68" s="77">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
         <v>208</v>
       </c>
@@ -5265,8 +5679,14 @@
       <c r="K69" s="78">
         <v>1453890.8941884842</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L69" s="78">
+        <v>1453890.8941884842</v>
+      </c>
+      <c r="M69" s="78">
+        <v>1453890.8941884842</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="17" t="s">
         <v>43</v>
       </c>
@@ -5300,8 +5720,14 @@
       <c r="K70" s="78">
         <v>1.3888888888888888E-5</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L70" s="78">
+        <v>1.3888888888888888E-5</v>
+      </c>
+      <c r="M70" s="78">
+        <v>1.3888888888888888E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
         <v>44</v>
       </c>
@@ -5335,8 +5761,14 @@
       <c r="K71" s="79">
         <v>6.5011574074074071E-4</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L71" s="79">
+        <v>6.5011574074074071E-4</v>
+      </c>
+      <c r="M71" s="79">
+        <v>6.5011574074074071E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
         <v>45</v>
       </c>
@@ -5370,8 +5802,14 @@
       <c r="K72" s="85">
         <v>4.7400000000000003E-3</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L72" s="85">
+        <v>4.7400000000000003E-3</v>
+      </c>
+      <c r="M72" s="85">
+        <v>4.7400000000000003E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="17" t="s">
         <v>46</v>
       </c>
@@ -5405,8 +5843,14 @@
       <c r="K73" s="79">
         <v>282528</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L73" s="79">
+        <v>282528</v>
+      </c>
+      <c r="M73" s="79">
+        <v>282528</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="17" t="s">
         <v>47</v>
       </c>
@@ -5440,8 +5884,14 @@
       <c r="K74" s="85">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L74" s="85">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M74" s="85">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
         <v>48</v>
       </c>
@@ -5475,8 +5925,14 @@
       <c r="K75" s="87">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L75" s="87">
+        <v>0.16</v>
+      </c>
+      <c r="M75" s="87">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="17" t="s">
         <v>49</v>
       </c>
@@ -5510,8 +5966,14 @@
       <c r="K76" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L76" s="77">
+        <v>0</v>
+      </c>
+      <c r="M76" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
         <v>50</v>
       </c>
@@ -5545,8 +6007,14 @@
       <c r="K77" s="78">
         <v>745476480000</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L77" s="78">
+        <v>745476480000</v>
+      </c>
+      <c r="M77" s="78">
+        <v>745476480000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
         <v>205</v>
       </c>
@@ -5580,8 +6048,14 @@
       <c r="K78" s="77">
         <v>100</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L78" s="77">
+        <v>100</v>
+      </c>
+      <c r="M78" s="77">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="33" t="s">
         <v>414</v>
       </c>
@@ -5615,8 +6089,14 @@
       <c r="K79" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L79" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="M79" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="33" t="s">
         <v>400</v>
       </c>
@@ -5650,8 +6130,14 @@
       <c r="K80" s="85">
         <v>21600</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L80" s="85">
+        <v>21600</v>
+      </c>
+      <c r="M80" s="85">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="33" t="s">
         <v>410</v>
       </c>
@@ -5685,8 +6171,14 @@
       <c r="K81" s="77">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L81" s="77">
+        <v>0.5</v>
+      </c>
+      <c r="M81" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="33" t="s">
         <v>401</v>
       </c>
@@ -5720,8 +6212,14 @@
       <c r="K82" s="85">
         <v>60479.999999999993</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L82" s="85">
+        <v>60479.999999999993</v>
+      </c>
+      <c r="M82" s="85">
+        <v>60479.999999999993</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="33" t="s">
         <v>411</v>
       </c>
@@ -5755,8 +6253,14 @@
       <c r="K83" s="77">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L83" s="77">
+        <v>0.85</v>
+      </c>
+      <c r="M83" s="77">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="33" t="s">
         <v>402</v>
       </c>
@@ -5790,8 +6294,14 @@
       <c r="K84" s="77">
         <v>518400</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L84" s="77">
+        <v>518400</v>
+      </c>
+      <c r="M84" s="77">
+        <v>518400</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="33" t="s">
         <v>412</v>
       </c>
@@ -5825,8 +6335,14 @@
       <c r="K85" s="77">
         <v>5184000</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L85" s="77">
+        <v>5184000</v>
+      </c>
+      <c r="M85" s="77">
+        <v>5184000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="17" t="s">
         <v>51</v>
       </c>
@@ -5860,8 +6376,14 @@
       <c r="K86" s="86">
         <v>50000</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L86" s="86">
+        <v>50000</v>
+      </c>
+      <c r="M86" s="86">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
         <v>52</v>
       </c>
@@ -5895,8 +6417,14 @@
       <c r="K87" s="77">
         <v>140000</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L87" s="77">
+        <v>140000</v>
+      </c>
+      <c r="M87" s="77">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
         <v>53</v>
       </c>
@@ -5930,8 +6458,14 @@
       <c r="K88" s="78">
         <v>3.6636136999999999E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L88" s="78">
+        <v>3.6636136999999999E-2</v>
+      </c>
+      <c r="M88" s="78">
+        <v>3.6636136999999999E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="17" t="s">
         <v>54</v>
       </c>
@@ -5965,8 +6499,14 @@
       <c r="K89" s="77">
         <v>4.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L89" s="77">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="M89" s="77">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="17" t="s">
         <v>55</v>
       </c>
@@ -6000,8 +6540,14 @@
       <c r="K90" s="77">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L90" s="77">
+        <v>0.05</v>
+      </c>
+      <c r="M90" s="77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="19" t="s">
         <v>214</v>
       </c>
@@ -6035,8 +6581,14 @@
       <c r="K91" s="77">
         <v>6.0000000000000002E-6</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L91" s="77">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="M91" s="77">
+        <v>6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="19" t="s">
         <v>215</v>
       </c>
@@ -6070,8 +6622,14 @@
       <c r="K92" s="77">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L92" s="77">
+        <v>0</v>
+      </c>
+      <c r="M92" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
         <v>216</v>
       </c>
@@ -6105,8 +6663,14 @@
       <c r="K93" s="77">
         <v>374999999.99999994</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L93" s="77">
+        <v>374999999.99999994</v>
+      </c>
+      <c r="M93" s="77">
+        <v>374999999.99999994</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>217</v>
       </c>
@@ -6140,8 +6704,14 @@
       <c r="K94" s="78">
         <v>3.7037037037037038E-3</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L94" s="78">
+        <v>3.7037037037037038E-3</v>
+      </c>
+      <c r="M94" s="78">
+        <v>3.7037037037037038E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="19" t="s">
         <v>218</v>
       </c>
@@ -6175,8 +6745,14 @@
       <c r="K95" s="77">
         <v>165600</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L95" s="77">
+        <v>165600</v>
+      </c>
+      <c r="M95" s="77">
+        <v>165600</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
         <v>60</v>
       </c>
@@ -6210,8 +6786,14 @@
       <c r="K96" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L96" s="77">
+        <v>20</v>
+      </c>
+      <c r="M96" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
         <v>209</v>
       </c>
@@ -6245,8 +6827,14 @@
       <c r="K97" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L97" s="77">
+        <v>1</v>
+      </c>
+      <c r="M97" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
         <v>59</v>
       </c>
@@ -6280,8 +6868,14 @@
       <c r="K98" s="77">
         <v>21</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L98" s="77">
+        <v>21</v>
+      </c>
+      <c r="M98" s="77">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="23" t="s">
         <v>65</v>
       </c>
@@ -6315,8 +6909,14 @@
       <c r="K99" s="77">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L99" s="77">
+        <v>0.64</v>
+      </c>
+      <c r="M99" s="77">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="23" t="s">
         <v>367</v>
       </c>
@@ -6350,8 +6950,14 @@
       <c r="K100" s="77">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L100" s="77">
+        <v>8</v>
+      </c>
+      <c r="M100" s="77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="23" t="s">
         <v>368</v>
       </c>
@@ -6385,8 +6991,14 @@
       <c r="K101" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L101" s="77">
+        <v>10</v>
+      </c>
+      <c r="M101" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="23" t="s">
         <v>369</v>
       </c>
@@ -6420,8 +7032,14 @@
       <c r="K102" s="77">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L102" s="77">
+        <v>8</v>
+      </c>
+      <c r="M102" s="77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="23" t="s">
         <v>505</v>
       </c>
@@ -6455,8 +7073,14 @@
       <c r="K103" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L103" s="77">
+        <v>1</v>
+      </c>
+      <c r="M103" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="23" t="s">
         <v>385</v>
       </c>
@@ -6490,8 +7114,14 @@
       <c r="K104" s="77">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L104" s="77">
+        <v>0.5</v>
+      </c>
+      <c r="M104" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="23" t="s">
         <v>506</v>
       </c>
@@ -6530,8 +7160,14 @@
         <f>K103</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L105" s="58">
+        <v>1</v>
+      </c>
+      <c r="M105" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="23" t="s">
         <v>507</v>
       </c>
@@ -6570,8 +7206,14 @@
         <f>150*K103</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L106" s="58">
+        <v>150</v>
+      </c>
+      <c r="M106" s="58">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="23" t="s">
         <v>508</v>
       </c>
@@ -6610,8 +7252,14 @@
         <f>K98</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L107" s="58">
+        <v>21</v>
+      </c>
+      <c r="M107" s="58">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="23" t="s">
         <v>509</v>
       </c>
@@ -6650,8 +7298,14 @@
         <f>70*K98</f>
         <v>1470</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L108" s="58">
+        <v>1470</v>
+      </c>
+      <c r="M108" s="58">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="23" t="s">
         <v>387</v>
       </c>
@@ -6685,8 +7339,14 @@
       <c r="K109" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L109" s="77">
+        <v>0</v>
+      </c>
+      <c r="M109" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="23" t="s">
         <v>389</v>
       </c>
@@ -6720,8 +7380,14 @@
       <c r="K110" s="82">
         <v>1589759.9999999998</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L110" s="82">
+        <v>1589759.9999999998</v>
+      </c>
+      <c r="M110" s="82">
+        <v>1589759.9999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="23" t="s">
         <v>391</v>
       </c>
@@ -6755,8 +7421,14 @@
       <c r="K111" s="82">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L111" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+      <c r="M111" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="23" t="s">
         <v>393</v>
       </c>
@@ -6790,8 +7462,14 @@
       <c r="K112" s="82">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L112" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+      <c r="M112" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="23" t="s">
         <v>421</v>
       </c>
@@ -6825,8 +7503,14 @@
       <c r="K113" s="82">
         <v>100</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L113" s="82">
+        <v>100</v>
+      </c>
+      <c r="M113" s="82">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="23" t="s">
         <v>423</v>
       </c>
@@ -6865,8 +7549,14 @@
         <f>0.1 * 3.25 * (60*60*24)</f>
         <v>28080</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L114" s="67">
+        <v>28080</v>
+      </c>
+      <c r="M114" s="67">
+        <v>28080</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="23" t="s">
         <v>425</v>
       </c>
@@ -6905,8 +7595,14 @@
         <f>1.11 / 10</f>
         <v>0.11100000000000002</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L115" s="67">
+        <v>0.11100000000000002</v>
+      </c>
+      <c r="M115" s="67">
+        <v>0.11100000000000002</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="23" t="s">
         <v>502</v>
       </c>
@@ -6940,8 +7636,14 @@
       <c r="K116" s="82">
         <v>100</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L116" s="82">
+        <v>100</v>
+      </c>
+      <c r="M116" s="82">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="23" t="s">
         <v>503</v>
       </c>
@@ -6980,8 +7682,14 @@
         <f>5.32 * (60*60*24)</f>
         <v>459648</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L117" s="67">
+        <v>459648</v>
+      </c>
+      <c r="M117" s="67">
+        <v>459648</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="23" t="s">
         <v>504</v>
       </c>
@@ -7020,8 +7728,14 @@
         <f>1.11/8</f>
         <v>0.13875000000000001</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L118" s="67">
+        <v>0.13875000000000001</v>
+      </c>
+      <c r="M118" s="67">
+        <v>0.13875000000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" s="23" t="s">
         <v>395</v>
       </c>
@@ -7055,8 +7769,14 @@
       <c r="K119" s="82">
         <v>21600</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L119" s="82">
+        <v>21600</v>
+      </c>
+      <c r="M119" s="82">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" s="23" t="s">
         <v>397</v>
       </c>
@@ -7090,8 +7810,14 @@
       <c r="K120" s="88">
         <v>43200</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L120" s="88">
+        <v>43200</v>
+      </c>
+      <c r="M120" s="88">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="13" t="s">
         <v>61</v>
       </c>
@@ -7125,8 +7851,14 @@
       <c r="K121" s="77">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L121" s="77">
+        <v>0.8</v>
+      </c>
+      <c r="M121" s="77">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="13" t="s">
         <v>62</v>
       </c>
@@ -7161,8 +7893,14 @@
       <c r="K122" s="78">
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L122" s="78">
+        <v>2.0833333333333335E-4</v>
+      </c>
+      <c r="M122" s="78">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="13" t="s">
         <v>63</v>
       </c>
@@ -7196,8 +7934,14 @@
       <c r="K123" s="77">
         <v>5.7899999999999998E-7</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L123" s="77">
+        <v>5.7899999999999998E-7</v>
+      </c>
+      <c r="M123" s="77">
+        <v>5.7899999999999998E-7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" s="13" t="s">
         <v>64</v>
       </c>
@@ -7231,8 +7975,14 @@
       <c r="K124" s="78">
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L124" s="78">
+        <v>2.0833333333333335E-4</v>
+      </c>
+      <c r="M124" s="78">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="13" t="s">
         <v>450</v>
       </c>
@@ -7266,8 +8016,14 @@
       <c r="K125" s="78">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L125" s="78">
+        <v>0</v>
+      </c>
+      <c r="M125" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" s="13" t="s">
         <v>452</v>
       </c>
@@ -7301,8 +8057,14 @@
       <c r="K126" s="78">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L126" s="78">
+        <v>0</v>
+      </c>
+      <c r="M126" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" s="68" t="s">
         <v>441</v>
       </c>
@@ -7334,8 +8096,14 @@
       <c r="K127" s="89">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L127" s="89">
+        <v>0</v>
+      </c>
+      <c r="M127" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="68" t="s">
         <v>67</v>
       </c>
@@ -7367,8 +8135,14 @@
       <c r="K128" s="89">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L128" s="89">
+        <v>0</v>
+      </c>
+      <c r="M128" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" s="68" t="s">
         <v>446</v>
       </c>
@@ -7402,8 +8176,14 @@
       <c r="K129" s="89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L129" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="M129" s="89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" s="21" t="s">
         <v>66</v>
       </c>
@@ -7437,8 +8217,14 @@
       <c r="K130" s="83">
         <v>5.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L130" s="83">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="M130" s="83">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" s="21" t="s">
         <v>438</v>
       </c>
@@ -7472,8 +8258,14 @@
       <c r="K131" s="83">
         <v>4.9999999999999999E-13</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L131" s="83">
+        <v>4.9999999999999999E-13</v>
+      </c>
+      <c r="M131" s="83">
+        <v>4.9999999999999999E-13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" s="21" t="s">
         <v>229</v>
       </c>
@@ -7507,8 +8299,14 @@
       <c r="K132" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L132" s="77">
+        <v>10</v>
+      </c>
+      <c r="M132" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" s="21" t="s">
         <v>230</v>
       </c>
@@ -7542,8 +8340,14 @@
       <c r="K133" s="77">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L133" s="77">
+        <v>-0.04</v>
+      </c>
+      <c r="M133" s="77">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" s="21" t="s">
         <v>231</v>
       </c>
@@ -7577,8 +8381,14 @@
       <c r="K134" s="77">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L134" s="77">
+        <v>2.9</v>
+      </c>
+      <c r="M134" s="77">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" s="21" t="s">
         <v>232</v>
       </c>
@@ -7612,8 +8422,14 @@
       <c r="K135" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L135" s="77">
+        <v>1</v>
+      </c>
+      <c r="M135" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" s="21" t="s">
         <v>68</v>
       </c>
@@ -7647,8 +8463,14 @@
       <c r="K136" s="80">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L136" s="80">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="M136" s="80">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" s="21" t="s">
         <v>233</v>
       </c>
@@ -7682,8 +8504,14 @@
       <c r="K137" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L137" s="77">
+        <v>10</v>
+      </c>
+      <c r="M137" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" s="21" t="s">
         <v>234</v>
       </c>
@@ -7717,8 +8545,14 @@
       <c r="K138" s="77">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L138" s="77">
+        <v>-0.04</v>
+      </c>
+      <c r="M138" s="77">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" s="21" t="s">
         <v>235</v>
       </c>
@@ -7752,8 +8586,14 @@
       <c r="K139" s="77">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L139" s="77">
+        <v>2.9</v>
+      </c>
+      <c r="M139" s="77">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" s="21" t="s">
         <v>236</v>
       </c>
@@ -7787,8 +8627,14 @@
       <c r="K140" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L140" s="77">
+        <v>1</v>
+      </c>
+      <c r="M140" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" s="21" t="s">
         <v>69</v>
       </c>
@@ -7822,8 +8668,14 @@
       <c r="K141" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L141" s="77">
+        <v>0</v>
+      </c>
+      <c r="M141" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" s="72" t="s">
         <v>70</v>
       </c>
@@ -7857,8 +8709,14 @@
       <c r="K142" s="80">
         <v>5.0000000000000004E-6</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L142" s="80">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="M142" s="80">
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" s="23" t="s">
         <v>56</v>
       </c>
@@ -7892,8 +8750,14 @@
       <c r="K143" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L143" s="77">
+        <v>0</v>
+      </c>
+      <c r="M143" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144" s="23" t="s">
         <v>57</v>
       </c>
@@ -7927,8 +8791,14 @@
       <c r="K144" s="77">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L144" s="77">
+        <v>2E-3</v>
+      </c>
+      <c r="M144" s="77">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145" s="23" t="s">
         <v>58</v>
       </c>
@@ -7962,8 +8832,14 @@
       <c r="K145" s="80">
         <v>3.9999999999999998E-6</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L145" s="80">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="M145" s="80">
+        <v>3.9999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146" s="23" t="s">
         <v>71</v>
       </c>
@@ -7997,8 +8873,14 @@
       <c r="K146" s="80">
         <v>3.7699999999999999E-10</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L146" s="80">
+        <v>3.7699999999999999E-10</v>
+      </c>
+      <c r="M146" s="80">
+        <v>3.7699999999999999E-10</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147" s="23" t="s">
         <v>237</v>
       </c>
@@ -8032,8 +8914,14 @@
       <c r="K147" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L147" s="77">
+        <v>20</v>
+      </c>
+      <c r="M147" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148" s="23" t="s">
         <v>238</v>
       </c>
@@ -8067,8 +8955,14 @@
       <c r="K148" s="77">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L148" s="77">
+        <v>-0.06</v>
+      </c>
+      <c r="M148" s="77">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149" s="23" t="s">
         <v>239</v>
       </c>
@@ -8102,8 +8996,14 @@
       <c r="K149" s="77">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L149" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="M149" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150" s="23" t="s">
         <v>240</v>
       </c>
@@ -8137,8 +9037,14 @@
       <c r="K150" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L150" s="77">
+        <v>1</v>
+      </c>
+      <c r="M150" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151" s="23" t="s">
         <v>72</v>
       </c>
@@ -8172,8 +9078,14 @@
       <c r="K151" s="80">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L151" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="M151" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152" s="13" t="s">
         <v>73</v>
       </c>
@@ -8207,8 +9119,14 @@
       <c r="K152" s="80">
         <v>5.8333333333333335E-9</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L152" s="80">
+        <v>5.8333333333333335E-9</v>
+      </c>
+      <c r="M152" s="80">
+        <v>5.8333333333333335E-9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153" s="13" t="s">
         <v>241</v>
       </c>
@@ -8242,8 +9160,14 @@
       <c r="K153" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L153" s="77">
+        <v>20</v>
+      </c>
+      <c r="M153" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154" s="13" t="s">
         <v>242</v>
       </c>
@@ -8277,8 +9201,14 @@
       <c r="K154" s="77">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L154" s="77">
+        <v>-0.06</v>
+      </c>
+      <c r="M154" s="77">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155" s="13" t="s">
         <v>243</v>
       </c>
@@ -8312,8 +9242,14 @@
       <c r="K155" s="77">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L155" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="M155" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156" s="13" t="s">
         <v>244</v>
       </c>
@@ -8347,8 +9283,14 @@
       <c r="K156" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L156" s="77">
+        <v>1</v>
+      </c>
+      <c r="M156" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157" s="13" t="s">
         <v>74</v>
       </c>
@@ -8382,8 +9324,14 @@
       <c r="K157" s="80">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L157" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="M157" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158" s="9" t="s">
         <v>75</v>
       </c>
@@ -8417,8 +9365,14 @@
       <c r="K158" s="83">
         <v>4.0000000000000001E-8</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L158" s="83">
+        <v>4.0000000000000001E-8</v>
+      </c>
+      <c r="M158" s="83">
+        <v>4.0000000000000001E-8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159" s="9" t="s">
         <v>219</v>
       </c>
@@ -8452,8 +9406,14 @@
       <c r="K159" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L159" s="77">
+        <v>20</v>
+      </c>
+      <c r="M159" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160" s="9" t="s">
         <v>220</v>
       </c>
@@ -8487,8 +9447,14 @@
       <c r="K160" s="77">
         <v>-4.4200000000000003E-2</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L160" s="77">
+        <v>-4.4200000000000003E-2</v>
+      </c>
+      <c r="M160" s="77">
+        <v>-4.4200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A161" s="9" t="s">
         <v>221</v>
       </c>
@@ -8522,8 +9488,14 @@
       <c r="K161" s="77">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L161" s="77">
+        <v>1.55</v>
+      </c>
+      <c r="M161" s="77">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A162" s="9" t="s">
         <v>222</v>
       </c>
@@ -8557,8 +9529,14 @@
       <c r="K162" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L162" s="77">
+        <v>1</v>
+      </c>
+      <c r="M162" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163" s="9" t="s">
         <v>76</v>
       </c>
@@ -8592,8 +9570,14 @@
       <c r="K163" s="77">
         <v>2.7799999999999998E-4</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L163" s="77">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="M163" s="77">
+        <v>2.7799999999999998E-4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164" s="25" t="s">
         <v>78</v>
       </c>
@@ -8630,8 +9614,14 @@
         <f>H164</f>
         <v>2.4999999999999998E-12</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L164" s="84">
+        <v>2.4999999999999998E-12</v>
+      </c>
+      <c r="M164" s="84">
+        <v>2.4999999999999998E-12</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165" s="25" t="s">
         <v>246</v>
       </c>
@@ -8665,8 +9655,14 @@
       <c r="K165" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L165" s="77">
+        <v>20</v>
+      </c>
+      <c r="M165" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166" s="25" t="s">
         <v>247</v>
       </c>
@@ -8700,8 +9696,14 @@
       <c r="K166" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L166" s="77">
+        <v>0</v>
+      </c>
+      <c r="M166" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167" s="25" t="s">
         <v>248</v>
       </c>
@@ -8735,8 +9737,14 @@
       <c r="K167" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L167" s="77">
+        <v>1</v>
+      </c>
+      <c r="M167" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A168" s="25" t="s">
         <v>249</v>
       </c>
@@ -8770,8 +9778,14 @@
       <c r="K168" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L168" s="77">
+        <v>0</v>
+      </c>
+      <c r="M168" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A169" s="25" t="s">
         <v>79</v>
       </c>
@@ -8805,8 +9819,14 @@
       <c r="K169" s="77">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L169" s="77">
+        <v>0.4</v>
+      </c>
+      <c r="M169" s="77">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170" s="31" t="s">
         <v>80</v>
       </c>
@@ -8840,8 +9860,14 @@
       <c r="K170" s="86">
         <v>2.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L170" s="86">
+        <v>2.0000000000000001E-9</v>
+      </c>
+      <c r="M170" s="86">
+        <v>2.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A171" s="31" t="s">
         <v>250</v>
       </c>
@@ -8875,8 +9901,14 @@
       <c r="K171" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L171" s="77">
+        <v>25</v>
+      </c>
+      <c r="M171" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172" s="31" t="s">
         <v>251</v>
       </c>
@@ -8910,8 +9942,14 @@
       <c r="K172" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L172" s="77">
+        <v>0</v>
+      </c>
+      <c r="M172" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173" s="31" t="s">
         <v>252</v>
       </c>
@@ -8945,8 +9983,14 @@
       <c r="K173" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L173" s="77">
+        <v>3.98</v>
+      </c>
+      <c r="M173" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A174" s="31" t="s">
         <v>253</v>
       </c>
@@ -8980,8 +10024,14 @@
       <c r="K174" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L174" s="77">
+        <v>1</v>
+      </c>
+      <c r="M174" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175" s="31" t="s">
         <v>81</v>
       </c>
@@ -9015,8 +10065,14 @@
       <c r="K175" s="78">
         <v>1.6666666666666666E-4</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L175" s="78">
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="M175" s="78">
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A176" s="11" t="s">
         <v>254</v>
       </c>
@@ -9050,8 +10106,14 @@
       <c r="K176" s="80">
         <v>1E-8</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L176" s="80">
+        <v>1E-8</v>
+      </c>
+      <c r="M176" s="80">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177" s="11" t="s">
         <v>255</v>
       </c>
@@ -9085,8 +10147,14 @@
       <c r="K177" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L177" s="77">
+        <v>20</v>
+      </c>
+      <c r="M177" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178" s="11" t="s">
         <v>256</v>
       </c>
@@ -9120,8 +10188,14 @@
       <c r="K178" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L178" s="77">
+        <v>0</v>
+      </c>
+      <c r="M178" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179" s="11" t="s">
         <v>257</v>
       </c>
@@ -9155,8 +10229,14 @@
       <c r="K179" s="77">
         <v>2</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L179" s="77">
+        <v>2</v>
+      </c>
+      <c r="M179" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180" s="11" t="s">
         <v>258</v>
       </c>
@@ -9190,8 +10270,14 @@
       <c r="K180" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L180" s="77">
+        <v>1</v>
+      </c>
+      <c r="M180" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181" s="11" t="s">
         <v>259</v>
       </c>
@@ -9225,8 +10311,14 @@
       <c r="K181" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L181" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="M181" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182" s="11" t="s">
         <v>260</v>
       </c>
@@ -9260,8 +10352,14 @@
       <c r="K182" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L182" s="77">
+        <v>1</v>
+      </c>
+      <c r="M182" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183" s="27" t="s">
         <v>261</v>
       </c>
@@ -9295,8 +10393,14 @@
       <c r="K183" s="77">
         <v>2.3533050791148899E-8</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L183" s="77">
+        <v>2.3533050791148899E-8</v>
+      </c>
+      <c r="M183" s="77">
+        <v>2.3533050791148899E-8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184" s="27" t="s">
         <v>262</v>
       </c>
@@ -9330,8 +10434,14 @@
       <c r="K184" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L184" s="77">
+        <v>20</v>
+      </c>
+      <c r="M184" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185" s="27" t="s">
         <v>263</v>
       </c>
@@ -9365,8 +10475,14 @@
       <c r="K185" s="77">
         <v>-0.187</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L185" s="77">
+        <v>-0.187</v>
+      </c>
+      <c r="M185" s="77">
+        <v>-0.187</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A186" s="27" t="s">
         <v>264</v>
       </c>
@@ -9400,8 +10516,14 @@
       <c r="K186" s="77">
         <v>2.48</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L186" s="77">
+        <v>2.48</v>
+      </c>
+      <c r="M186" s="77">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187" s="27" t="s">
         <v>265</v>
       </c>
@@ -9435,8 +10557,14 @@
       <c r="K187" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L187" s="77">
+        <v>1</v>
+      </c>
+      <c r="M187" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188" s="27" t="s">
         <v>266</v>
       </c>
@@ -9470,8 +10598,14 @@
       <c r="K188" s="77">
         <v>6.1060227588121015E-4</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L188" s="77">
+        <v>6.1060227588121015E-4</v>
+      </c>
+      <c r="M188" s="77">
+        <v>6.1060227588121015E-4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189" s="23" t="s">
         <v>267</v>
       </c>
@@ -9505,8 +10639,14 @@
       <c r="K189" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L189" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="M189" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190" s="23" t="s">
         <v>268</v>
       </c>
@@ -9540,8 +10680,14 @@
       <c r="K190" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L190" s="77">
+        <v>25</v>
+      </c>
+      <c r="M190" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191" s="23" t="s">
         <v>269</v>
       </c>
@@ -9575,8 +10721,14 @@
       <c r="K191" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L191" s="77">
+        <v>0</v>
+      </c>
+      <c r="M191" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192" s="23" t="s">
         <v>270</v>
       </c>
@@ -9610,8 +10762,14 @@
       <c r="K192" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L192" s="77">
+        <v>3.98</v>
+      </c>
+      <c r="M192" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193" s="23" t="s">
         <v>271</v>
       </c>
@@ -9645,8 +10803,14 @@
       <c r="K193" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L193" s="77">
+        <v>1</v>
+      </c>
+      <c r="M193" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194" s="23" t="s">
         <v>272</v>
       </c>
@@ -9680,8 +10844,14 @@
       <c r="K194" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L194" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="M194" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
         <v>273</v>
       </c>
@@ -9715,8 +10885,14 @@
       <c r="K195" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L195" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="M195" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>274</v>
       </c>
@@ -9750,8 +10926,14 @@
       <c r="K196" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L196" s="77">
+        <v>25</v>
+      </c>
+      <c r="M196" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>275</v>
       </c>
@@ -9785,8 +10967,14 @@
       <c r="K197" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L197" s="77">
+        <v>0</v>
+      </c>
+      <c r="M197" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
         <v>276</v>
       </c>
@@ -9820,8 +11008,14 @@
       <c r="K198" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L198" s="77">
+        <v>3.98</v>
+      </c>
+      <c r="M198" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
         <v>277</v>
       </c>
@@ -9855,8 +11049,14 @@
       <c r="K199" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L199" s="77">
+        <v>1</v>
+      </c>
+      <c r="M199" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
         <v>278</v>
       </c>
@@ -9890,8 +11090,14 @@
       <c r="K200" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L200" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="M200" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201" s="29" t="s">
         <v>279</v>
       </c>
@@ -9925,8 +11131,14 @@
       <c r="K201" s="85">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L201" s="85">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="M201" s="85">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202" s="29" t="s">
         <v>280</v>
       </c>
@@ -9960,8 +11172,14 @@
       <c r="K202" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L202" s="77">
+        <v>25</v>
+      </c>
+      <c r="M202" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203" s="29" t="s">
         <v>281</v>
       </c>
@@ -9995,8 +11213,14 @@
       <c r="K203" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L203" s="77">
+        <v>0</v>
+      </c>
+      <c r="M203" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204" s="29" t="s">
         <v>282</v>
       </c>
@@ -10030,8 +11254,14 @@
       <c r="K204" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L204" s="77">
+        <v>3.98</v>
+      </c>
+      <c r="M204" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205" s="29" t="s">
         <v>283</v>
       </c>
@@ -10065,8 +11295,14 @@
       <c r="K205" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L205" s="77">
+        <v>1</v>
+      </c>
+      <c r="M205" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206" s="29" t="s">
         <v>284</v>
       </c>
@@ -10100,8 +11336,14 @@
       <c r="K206" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L206" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="M206" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207" s="90" t="s">
         <v>362</v>
       </c>
@@ -10135,8 +11377,14 @@
       <c r="K207" s="95" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L207" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="M207" s="95" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>495</v>
       </c>
@@ -10170,8 +11418,14 @@
       <c r="K208" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L208" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="M208" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>499</v>
       </c>
@@ -10205,8 +11459,14 @@
       <c r="K209" s="99">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L209" s="99">
+        <v>0</v>
+      </c>
+      <c r="M209" s="99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>522</v>
       </c>
@@ -10244,8 +11504,14 @@
         <f>K209</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L210" s="99">
+        <v>0</v>
+      </c>
+      <c r="M210" s="99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>513</v>
       </c>
@@ -10279,8 +11545,14 @@
       <c r="K211" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L211" s="100">
+        <v>1</v>
+      </c>
+      <c r="M211" s="100">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>514</v>
       </c>
@@ -10314,8 +11586,14 @@
       <c r="K212" s="98" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L212" s="98">
+        <v>0.1</v>
+      </c>
+      <c r="M212" s="98" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>515</v>
       </c>
@@ -10349,8 +11627,14 @@
       <c r="K213" s="98">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L213" s="98">
+        <v>0.04</v>
+      </c>
+      <c r="M213" s="98">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>516</v>
       </c>
@@ -10384,8 +11668,14 @@
       <c r="K214" s="98">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L214" s="98">
+        <v>1E-3</v>
+      </c>
+      <c r="M214" s="98">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>526</v>
       </c>
@@ -10419,8 +11709,14 @@
       <c r="K215" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L215" s="2">
+        <v>29</v>
+      </c>
+      <c r="M215" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>528</v>
       </c>
@@ -10459,8 +11755,14 @@
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-4</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L216" s="99">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="M216" s="99">
+        <v>2.5000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>531</v>
       </c>
@@ -10494,8 +11796,14 @@
       <c r="K217" s="100">
         <v>9.9999999999999994E-12</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L217" s="100">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="M217" s="100">
+        <v>9.9999999999999994E-12</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>534</v>
       </c>
@@ -10529,10 +11837,16 @@
       <c r="K218" s="99">
         <v>2.0000000000000001E-4</v>
       </c>
+      <c r="L218" s="99">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="M218" s="99">
+        <v>2.0000000000000001E-4</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H125:K126">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10543,17 +11857,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H130:K130">
-    <cfRule type="colorScale" priority="228">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="H130:M130">
     <cfRule type="colorScale" priority="229">
       <colorScale>
         <cfvo type="min"/>
@@ -10564,8 +11868,6 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H131:K131">
     <cfRule type="colorScale" priority="230">
       <colorScale>
         <cfvo type="min"/>
@@ -10576,6 +11878,8 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H131:M131">
     <cfRule type="colorScale" priority="231">
       <colorScale>
         <cfvo type="min"/>
@@ -10586,8 +11890,6 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H136:K136">
     <cfRule type="colorScale" priority="232">
       <colorScale>
         <cfvo type="min"/>
@@ -10599,7 +11901,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H142:K142">
+  <conditionalFormatting sqref="H136:M136">
     <cfRule type="colorScale" priority="233">
       <colorScale>
         <cfvo type="min"/>
@@ -10610,6 +11912,8 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H142:M142">
     <cfRule type="colorScale" priority="234">
       <colorScale>
         <cfvo type="min"/>
@@ -10630,8 +11934,6 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H158:K158">
     <cfRule type="colorScale" priority="236">
       <colorScale>
         <cfvo type="min"/>
@@ -10642,6 +11944,8 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H158:M158">
     <cfRule type="colorScale" priority="237">
       <colorScale>
         <cfvo type="min"/>
@@ -10662,8 +11966,6 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H164:K164">
     <cfRule type="colorScale" priority="239">
       <colorScale>
         <cfvo type="min"/>
@@ -10674,6 +11976,8 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H164:M164">
     <cfRule type="colorScale" priority="240">
       <colorScale>
         <cfvo type="min"/>
@@ -10685,6 +11989,28 @@
       </colorScale>
     </cfRule>
     <cfRule type="colorScale" priority="241">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="242">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L125:M126">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>